<commit_message>
little front changes as training
</commit_message>
<xml_diff>
--- a/Organization/Gantt.xlsx
+++ b/Organization/Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\4IIR\PFA\Organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\4IIR\PFA\PFA_Ecommerce\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E80C30-99D4-445A-B0B3-6E617EE82507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6B0958-364E-4783-9506-88D422C0DF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -120,21 +119,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,13 +413,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,92 +439,97 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="e">
-        <f>B2+C2</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>44596</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>